<commit_message>
Tabelas para corrigir OBM
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Vocabulários EDQM/unidadesdeapresentação.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Vocabulários EDQM/unidadesdeapresentação.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Library/CloudStorage/GoogleDrive-jussara.macedo@gmail.com/Meu Drive/SIRIOSCT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Vocabulários EDQM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{133CE7E3-2D0B-654D-BC45-FFC0B5BBD666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46832F8B-C828-9748-B3B4-C4964C0CF03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D631FA23-FD0B-4746-A4FF-17B0928A1D1C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17860" xr2:uid="{D631FA23-FD0B-4746-A4FF-17B0928A1D1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -785,6 +785,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>